<commit_message>
Exporting to excel and downloading the file
</commit_message>
<xml_diff>
--- a/ExpenseTracker_Backend/expenses_2024_2.xlsx
+++ b/ExpenseTracker_Backend/expenses_2024_2.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>ID</t>
+    <t>Expense Date</t>
   </si>
   <si>
     <t>Expense Value</t>
@@ -23,16 +23,13 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Expense Date</t>
-  </si>
-  <si>
     <t>Expense Type</t>
   </si>
   <si>
-    <t>New 01</t>
+    <t>2024-02-04</t>
   </si>
   <si>
-    <t>2024-02-04</t>
+    <t>New 01</t>
   </si>
   <si>
     <t>OTHER</t>
@@ -80,7 +77,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -99,13 +96,10 @@
       <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
-        <v>4</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>13.0</v>
+      <c r="A2" t="s" s="0">
+        <v>4</v>
       </c>
       <c r="B2" t="n" s="0">
         <v>100.0</v>
@@ -116,9 +110,6 @@
       <c r="D2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="E2" t="s" s="0">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>